<commit_message>
Move the simulation results to correct location.
</commit_message>
<xml_diff>
--- a/results/simulation-results-table.xlsx
+++ b/results/simulation-results-table.xlsx
@@ -1,25 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27211"/>
+  <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ppml_simulation\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/errard/Dropbox/GitHub/ppml_simulation/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14295" windowHeight="10650"/>
+    <workbookView xWindow="13740" yWindow="560" windowWidth="20360" windowHeight="18640"/>
   </bookViews>
   <sheets>
     <sheet name="simulation-results-2018-08-14" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>fixed effects</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -65,32 +73,107 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Model 1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Model 2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Note: the results are based on 1,000 simulations.</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Model 3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Model 4</t>
+    <t>(1)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>(2)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>(3)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>(4)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPML Monte Carlo Simulation Results with Different Fixexd Effect Settings</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Note: the results are based on 1,000 simulations. Column (1) and (3) show the simulation results based on models which drop one importer fixed effect each year. Column (2) and (4) show those based on models drop only one importer fixed effect. The mean error of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>var</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2 in Column (4) is -0.0000030. The true values of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>var</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1 and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>var</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2 are 1 and -1, respectively.</t>
+    </r>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="0.0000000_ "/>
+    <numFmt numFmtId="176" formatCode="0.0000_ "/>
   </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
@@ -270,10 +353,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="新細明體"/>
-      <family val="1"/>
+      <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
@@ -459,7 +543,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -578,7 +662,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -588,7 +672,18 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -721,7 +816,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -743,20 +838,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -780,18 +884,17 @@
     <cellStyle name="60% - 輔色6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="中等" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="合計" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="計算方式" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="計算" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="連結的儲存格" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="備註" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="說明文字" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="輔色1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="輔色2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="輔色3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="輔色4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="輔色5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="輔色6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="輔色 1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="輔色 2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="輔色 3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="輔色 4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="輔色 5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="輔色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="標題" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="標題 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="標題 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -800,6 +903,7 @@
     <cellStyle name="輸入" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="輸出" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="檢查儲存格" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="總計" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="壞" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="警告文字" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
@@ -1079,231 +1183,288 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="172" zoomScalePageLayoutView="172" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="19.875" style="1" customWidth="1"/>
-    <col min="2" max="5" width="10.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" style="1" customWidth="1"/>
+    <col min="2" max="5" width="10.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B5" s="3">
         <v>-2.9999999999999997E-4</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C5" s="3">
         <v>-1.6000000000000001E-3</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="10">
-        <v>-5.6999999999999998E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="D5" s="8">
+        <v>-1E-3</v>
+      </c>
+      <c r="E5" s="9">
+        <v>-5.6970000000000002E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B6" s="3">
         <v>2.3E-3</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C6" s="3">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="10">
-        <v>-2.5900000000000002E-6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="4"/>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="D6" s="8">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="E6" s="9">
+        <v>-3.0000000000000001E-6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="4"/>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="B8" s="3"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B10" s="3">
         <v>3.8699999999999998E-2</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C10" s="3">
         <v>3.9600000000000003E-2</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="10">
-        <v>2.1577117999999999E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="D10" s="8">
+        <v>2.1600000000000001E-2</v>
+      </c>
+      <c r="E10" s="9">
+        <v>2.1600000000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B11" s="3">
         <v>3.9600000000000003E-2</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C11" s="3">
         <v>3.9699999999999999E-2</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="10">
-        <v>2.1505654999999999E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="D11" s="8">
+        <v>2.1299999999999999E-2</v>
+      </c>
+      <c r="E11" s="9">
+        <v>2.1499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B13" s="12">
         <v>500</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C13" s="12">
         <v>500</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9">
+      <c r="D13" s="12">
         <v>1000</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="E13" s="12">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-    </row>
-    <row r="14" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+    </row>
+    <row r="15" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B16" s="12">
         <v>490</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C16" s="12">
         <v>499</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9">
+      <c r="D16" s="12">
+        <v>990</v>
+      </c>
+      <c r="E16" s="12">
         <v>999</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-    </row>
-    <row r="17" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+    </row>
+    <row r="18" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B19" s="1">
         <v>50</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C19" s="1">
         <v>50</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4">
+      <c r="D19" s="4">
         <v>100</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="E19" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B20" s="1">
         <v>10</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C20" s="1">
         <v>10</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11">
+      <c r="D20" s="7">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-    </row>
-    <row r="22" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="E20" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+    </row>
+    <row r="25" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="26" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C15:C16"/>
+  <mergeCells count="10">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A21:E24"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C16:C17"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>